<commit_message>
fix name and update debug log
</commit_message>
<xml_diff>
--- a/manual_debug_log/used_tools.xlsx
+++ b/manual_debug_log/used_tools.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcma/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcma/asplos22-hardware-debugging-artifact/hardware-bugbase/manual_debug_log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0642CA-ADB0-4741-8527-43ABF6BA5117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B440B9-88E0-844F-BEA0-448DA8C159FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51200" yWindow="-2580" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="93">
   <si>
     <t>Debugging Helpers</t>
   </si>
@@ -238,12 +237,6 @@
     </r>
   </si>
   <si>
-    <t>D8-Failure-to-Reset-SHA512</t>
-  </si>
-  <si>
-    <t>D4-Bit-Truncation-SHA512</t>
-  </si>
-  <si>
     <t>D1-Buffer-Overflow-RSD</t>
   </si>
   <si>
@@ -262,21 +255,9 @@
     <t>S2-Protocol-Violation-AXI-Stream</t>
   </si>
   <si>
-    <t>C3-Data-Control-Asynchrony-SDSPI</t>
-  </si>
-  <si>
     <t>C1-Dead-Lock-SDSPI</t>
   </si>
   <si>
-    <t>D7-Endianness-Mismatch-SDSPI</t>
-  </si>
-  <si>
-    <t>D5-Bit-Truncation-FFT</t>
-  </si>
-  <si>
-    <t>D6-Misindexing-FADD</t>
-  </si>
-  <si>
     <t>SignalCat(input at each stage)</t>
   </si>
   <si>
@@ -290,6 +271,123 @@
   </si>
   <si>
     <t>protocol violated</t>
+  </si>
+  <si>
+    <t>C3-Signal-Asynchrony-SDSPI</t>
+  </si>
+  <si>
+    <t>D4-Buffer-Overflow-Frame-FIFO</t>
+  </si>
+  <si>
+    <t>StatisticsMonitor(axis_fifo_inst.s_axis_tlast)
+StatisticsMonitor(axis_fifo_inst.m_axis_tlast)</t>
+  </si>
+  <si>
+    <t>The number of input frames and output frames are not equal. Something is lost in the middle.</t>
+  </si>
+  <si>
+    <t>SignalCat(axis_fifo_inst.write)
+SignalCat(axis_fifo_inst.wr_addr_reg)</t>
+  </si>
+  <si>
+    <t>wr_addr_reg behaves weird, and the logic to update it is problematic</t>
+  </si>
+  <si>
+    <t>D5-Bit-Truncation-SHA512</t>
+  </si>
+  <si>
+    <t>D6-Bit-Truncation-FFT</t>
+  </si>
+  <si>
+    <t>D7-Misindexing-FADD</t>
+  </si>
+  <si>
+    <t>D8-Misindexing-AXIS-Switch</t>
+  </si>
+  <si>
+    <t>SignalCat(s_axis_tvalid[3:0])
+SignalCat(s_axis_tready[3:0])
+SignalCat(m_axis_tvalid)
+SignalCat(m_axis_tready)</t>
+  </si>
+  <si>
+    <t>The input's ready bit does not match with expectation.</t>
+  </si>
+  <si>
+    <t>SignalCat(UUT.int_axis_tready[3:0])</t>
+  </si>
+  <si>
+    <t>The value of int_axis_tready is wrong, which indicates the logic passes the control to a wrong port. A deeper inspection would find the misindexing.</t>
+  </si>
+  <si>
+    <t>D9-Endianness-Mismatch-SDSPI</t>
+  </si>
+  <si>
+    <t>D10-Failure-to-Update-SHA512</t>
+  </si>
+  <si>
+    <t>D11-Failure-to-Update-Frame-FIFO</t>
+  </si>
+  <si>
+    <t>D12-Failure-to-Update-Frame-FIFO</t>
+  </si>
+  <si>
+    <t>D13-Failure-to-Update-Frame-Length-Measurer</t>
+  </si>
+  <si>
+    <t>DependencyMonitor(drop_frame, 1)</t>
+  </si>
+  <si>
+    <t>The failure-to-update of the drop_frame variable can be located</t>
+  </si>
+  <si>
+    <t>DependencyMonitor(drop_frame_reg, 1)
+DependencyMonitor(drop_frame_next, 1)
+DependencyMonitor(full_cur, 1)
+DependencyMonitor(full_wr, 1)</t>
+  </si>
+  <si>
+    <t>drop_frame_reg is not consistant in a frame, investigation shows it's a failure-to-update bug.</t>
+  </si>
+  <si>
+    <t>StatisticsMonitor(frame_reg[0])</t>
+  </si>
+  <si>
+    <t>The count of frame does not match expectation.</t>
+  </si>
+  <si>
+    <t>DependencyMonitor(frame_len_reg[15:0], 1)
+DependencyMonitor(frame_len_next[15:0], 1)</t>
+  </si>
+  <si>
+    <t>The frame_len_reg register is not cleared during reset.</t>
+  </si>
+  <si>
+    <t>C4-Signal-Asynchrony-AXI-Stream-FIFO</t>
+  </si>
+  <si>
+    <t>SignalCat(async_rst)
+SignalCat(reg_axis_tvalid)
+SignalCat(reg_axis_tready)
+SignalCat(reg_axis_tlast)
+SignalCat(UUT.full)
+SignalCat(UUT.empty)
+SignalCat(UUT.write)
+SignalCat(UUT.read)</t>
+  </si>
+  <si>
+    <t>In a cycle after reset, UUT.write is 0 but the circuit is accepting packet. A deeper inspection can find that the reset signal arrives 1 cycle slower than data.</t>
+  </si>
+  <si>
+    <t>S3-Incomple-Implementation-AXIS-Adapter</t>
+  </si>
+  <si>
+    <t>SignalCat(output_axis_tlast_int)
+SignalCat(input_axis_tlast)
+SignalCat(input_axis_tkeep)</t>
+  </si>
+  <si>
+    <t>The occurrence of tlast is not correct. Input's tkeep shows an unhandled case.</t>
   </si>
 </sst>
 </file>
@@ -450,7 +548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -537,6 +635,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -762,16 +864,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W997"/>
+  <dimension ref="A1:W1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="34.6640625" customWidth="1"/>
-    <col min="2" max="2" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" customWidth="1"/>
     <col min="3" max="3" width="38" style="23" customWidth="1"/>
     <col min="4" max="4" width="40.6640625" style="23" customWidth="1"/>
     <col min="5" max="5" width="36.5" customWidth="1"/>
@@ -915,7 +1017,7 @@
     </row>
     <row r="7" spans="1:23" ht="56">
       <c r="A7" s="34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>31</v>
@@ -940,7 +1042,7 @@
     </row>
     <row r="8" spans="1:23" ht="84">
       <c r="A8" s="34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>31</v>
@@ -961,7 +1063,7 @@
     </row>
     <row r="9" spans="1:23" ht="98">
       <c r="A9" s="19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>32</v>
@@ -988,63 +1090,67 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="56">
-      <c r="A10" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="25" t="s">
+    <row r="10" spans="1:23" ht="28">
+      <c r="A10" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+    </row>
+    <row r="11" spans="1:23" ht="56">
+      <c r="A11" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C11" s="22" t="s">
         <v>14</v>
-      </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-    </row>
-    <row r="11" spans="1:23" ht="98">
-      <c r="A11" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>26</v>
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="36"/>
-      <c r="F11" s="35"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="36"/>
-      <c r="H11" s="35"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="36"/>
-    </row>
-    <row r="12" spans="1:23" ht="42">
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
+    </row>
+    <row r="12" spans="1:23" ht="98">
       <c r="A12" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>24</v>
+        <v>67</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="36"/>
@@ -1053,15 +1159,15 @@
       <c r="H12" s="35"/>
       <c r="I12" s="36"/>
     </row>
-    <row r="13" spans="1:23" ht="28">
+    <row r="13" spans="1:23" ht="42">
       <c r="A13" s="34" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>25</v>
+      <c r="C13" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="D13" s="37"/>
       <c r="E13" s="36"/>
@@ -1071,162 +1177,253 @@
       <c r="I13" s="36"/>
     </row>
     <row r="14" spans="1:23" ht="56">
-      <c r="A14" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>15</v>
+      <c r="A14" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="36"/>
       <c r="H14" s="35"/>
       <c r="I14" s="36"/>
     </row>
-    <row r="15" spans="1:23" ht="14">
+    <row r="15" spans="1:23" ht="28">
       <c r="A15" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>63</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="37"/>
+      <c r="E15" s="36"/>
       <c r="F15" s="35"/>
       <c r="G15" s="36"/>
       <c r="H15" s="35"/>
       <c r="I15" s="36"/>
     </row>
-    <row r="16" spans="1:23" ht="98">
-      <c r="A16" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>32</v>
+    <row r="16" spans="1:23" ht="56">
+      <c r="A16" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>46</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>40</v>
+        <v>14</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>33</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="56">
-      <c r="A17" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="37"/>
-      <c r="E17" s="36"/>
+        <v>15</v>
+      </c>
+      <c r="F16" s="35"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="36"/>
+    </row>
+    <row r="17" spans="1:9" ht="28">
+      <c r="A17" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
       <c r="F17" s="35"/>
       <c r="G17" s="36"/>
       <c r="H17" s="35"/>
       <c r="I17" s="36"/>
     </row>
-    <row r="18" spans="1:9" ht="14">
-      <c r="A18" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="36"/>
+    <row r="18" spans="1:9" ht="56">
+      <c r="A18" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
       <c r="F18" s="35"/>
       <c r="G18" s="36"/>
       <c r="H18" s="35"/>
       <c r="I18" s="36"/>
     </row>
-    <row r="19" spans="1:9" ht="14">
-      <c r="A19" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="36"/>
+    <row r="19" spans="1:9" ht="28">
+      <c r="A19" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>86</v>
+      </c>
       <c r="F19" s="35"/>
       <c r="G19" s="36"/>
       <c r="H19" s="35"/>
       <c r="I19" s="36"/>
     </row>
-    <row r="23" spans="1:9" ht="13">
-      <c r="B23" s="12"/>
-      <c r="D23" s="10"/>
-      <c r="F23" s="9"/>
-      <c r="H23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" ht="13">
-      <c r="B24" s="12"/>
-      <c r="D24" s="10"/>
-      <c r="F24" s="9"/>
-      <c r="H24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" ht="13">
-      <c r="B25" s="12"/>
-      <c r="D25" s="10"/>
-      <c r="F25" s="9"/>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" ht="13">
-      <c r="B26" s="12"/>
-      <c r="D26" s="10"/>
-      <c r="F26" s="9"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" ht="13">
-      <c r="B27" s="12"/>
-      <c r="D27" s="10"/>
-      <c r="F27" s="9"/>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" ht="13">
-      <c r="B28" s="12"/>
-      <c r="D28" s="10"/>
-      <c r="F28" s="9"/>
-      <c r="H28" s="9"/>
+    <row r="20" spans="1:9" ht="14">
+      <c r="A20" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="35"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="36"/>
+    </row>
+    <row r="21" spans="1:9" ht="98">
+      <c r="A21" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="56">
+      <c r="A22" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="37"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="36"/>
+    </row>
+    <row r="23" spans="1:9" ht="112">
+      <c r="A23" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="37"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="36"/>
+    </row>
+    <row r="24" spans="1:9" ht="14">
+      <c r="A24" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="37"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="36"/>
+    </row>
+    <row r="25" spans="1:9" ht="14">
+      <c r="A25" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="37"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="36"/>
+    </row>
+    <row r="26" spans="1:9" ht="52" customHeight="1">
+      <c r="A26" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="35"/>
     </row>
     <row r="29" spans="1:9" ht="13">
       <c r="B29" s="12"/>
@@ -7042,6 +7239,42 @@
       <c r="F997" s="9"/>
       <c r="H997" s="9"/>
     </row>
+    <row r="998" spans="2:8" ht="13">
+      <c r="B998" s="12"/>
+      <c r="D998" s="10"/>
+      <c r="F998" s="9"/>
+      <c r="H998" s="9"/>
+    </row>
+    <row r="999" spans="2:8" ht="13">
+      <c r="B999" s="12"/>
+      <c r="D999" s="10"/>
+      <c r="F999" s="9"/>
+      <c r="H999" s="9"/>
+    </row>
+    <row r="1000" spans="2:8" ht="13">
+      <c r="B1000" s="12"/>
+      <c r="D1000" s="10"/>
+      <c r="F1000" s="9"/>
+      <c r="H1000" s="9"/>
+    </row>
+    <row r="1001" spans="2:8" ht="13">
+      <c r="B1001" s="12"/>
+      <c r="D1001" s="10"/>
+      <c r="F1001" s="9"/>
+      <c r="H1001" s="9"/>
+    </row>
+    <row r="1002" spans="2:8" ht="13">
+      <c r="B1002" s="12"/>
+      <c r="D1002" s="10"/>
+      <c r="F1002" s="9"/>
+      <c r="H1002" s="9"/>
+    </row>
+    <row r="1003" spans="2:8" ht="13">
+      <c r="B1003" s="12"/>
+      <c r="D1003" s="10"/>
+      <c r="F1003" s="9"/>
+      <c r="H1003" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>